<commit_message>
Cloud Stage -Wave 1 2023 Run - 138 test cases
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics_CRM_Cloud_2023_Wave1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FC4653-7461-4E0F-80B0-03FF1D3A87FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F68E06-7385-4707-BDE6-A3A9FD936CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -6781,8 +6781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
   <dimension ref="A1:P318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7947,8 +7947,8 @@
       <c r="B40" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="C40" s="132" t="s">
-        <v>32</v>
+      <c r="C40" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>1</v>
@@ -7975,8 +7975,8 @@
       <c r="B41" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="C41" s="132" t="s">
-        <v>32</v>
+      <c r="C41" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>1</v>
@@ -8003,8 +8003,8 @@
       <c r="B42" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="C42" s="132" t="s">
-        <v>32</v>
+      <c r="C42" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>1</v>
@@ -8031,8 +8031,8 @@
       <c r="B43" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="C43" s="132" t="s">
-        <v>32</v>
+      <c r="C43" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>1</v>
@@ -8059,8 +8059,8 @@
       <c r="B44" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="C44" s="132" t="s">
-        <v>32</v>
+      <c r="C44" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>1</v>
@@ -8087,8 +8087,8 @@
       <c r="B45" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="C45" s="132" t="s">
-        <v>32</v>
+      <c r="C45" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>1</v>
@@ -8115,8 +8115,8 @@
       <c r="B46" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="C46" s="132" t="s">
-        <v>32</v>
+      <c r="C46" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>1</v>
@@ -8143,8 +8143,8 @@
       <c r="B47" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="C47" s="132" t="s">
-        <v>32</v>
+      <c r="C47" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>1</v>
@@ -8171,8 +8171,8 @@
       <c r="B48" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="C48" s="132" t="s">
-        <v>32</v>
+      <c r="C48" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>1</v>
@@ -8199,8 +8199,8 @@
       <c r="B49" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="C49" s="132" t="s">
-        <v>32</v>
+      <c r="C49" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D49" s="17" t="s">
         <v>1</v>
@@ -8227,8 +8227,8 @@
       <c r="B50" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="C50" s="132" t="s">
-        <v>32</v>
+      <c r="C50" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>1</v>
@@ -8255,8 +8255,8 @@
       <c r="B51" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="C51" s="132" t="s">
-        <v>32</v>
+      <c r="C51" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D51" s="17" t="s">
         <v>1</v>
@@ -8284,7 +8284,7 @@
         <v>542</v>
       </c>
       <c r="C52" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D52" s="17" t="s">
         <v>1</v>
@@ -8312,7 +8312,7 @@
         <v>544</v>
       </c>
       <c r="C53" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D53" s="17" t="s">
         <v>1</v>
@@ -8339,8 +8339,8 @@
       <c r="B54" s="41" t="s">
         <v>546</v>
       </c>
-      <c r="C54" s="126" t="s">
-        <v>32</v>
+      <c r="C54" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>1</v>
@@ -8368,7 +8368,7 @@
         <v>550</v>
       </c>
       <c r="C55" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>1</v>
@@ -8396,7 +8396,7 @@
         <v>552</v>
       </c>
       <c r="C56" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>1</v>
@@ -8426,7 +8426,7 @@
         <v>554</v>
       </c>
       <c r="C57" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D57" s="17" t="s">
         <v>1</v>
@@ -8456,7 +8456,7 @@
         <v>555</v>
       </c>
       <c r="C58" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D58" s="17" t="s">
         <v>1</v>
@@ -8484,7 +8484,7 @@
         <v>558</v>
       </c>
       <c r="C59" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D59" s="17" t="s">
         <v>1</v>
@@ -8514,7 +8514,7 @@
         <v>560</v>
       </c>
       <c r="C60" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D60" s="17" t="s">
         <v>1</v>
@@ -8544,7 +8544,7 @@
         <v>562</v>
       </c>
       <c r="C61" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D61" s="17" t="s">
         <v>1</v>
@@ -8574,7 +8574,7 @@
         <v>564</v>
       </c>
       <c r="C62" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D62" s="17" t="s">
         <v>1</v>
@@ -8604,7 +8604,7 @@
         <v>566</v>
       </c>
       <c r="C63" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D63" s="17" t="s">
         <v>1</v>
@@ -8632,7 +8632,7 @@
         <v>568</v>
       </c>
       <c r="C64" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>1</v>
@@ -8662,7 +8662,7 @@
         <v>571</v>
       </c>
       <c r="C65" s="146" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D65" s="17" t="s">
         <v>1</v>
@@ -8690,7 +8690,7 @@
         <v>573</v>
       </c>
       <c r="C66" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D66" s="17" t="s">
         <v>1</v>
@@ -8718,7 +8718,7 @@
         <v>575</v>
       </c>
       <c r="C67" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D67" s="17" t="s">
         <v>1</v>
@@ -8744,7 +8744,7 @@
         <v>577</v>
       </c>
       <c r="C68" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D68" s="17" t="s">
         <v>1</v>
@@ -8770,7 +8770,7 @@
         <v>579</v>
       </c>
       <c r="C69" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D69" s="17" t="s">
         <v>1</v>
@@ -8796,7 +8796,7 @@
         <v>582</v>
       </c>
       <c r="C70" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D70" s="17" t="s">
         <v>1</v>
@@ -8823,8 +8823,8 @@
       <c r="B71" s="15" t="s">
         <v>583</v>
       </c>
-      <c r="C71" s="126" t="s">
-        <v>32</v>
+      <c r="C71" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D71" s="17" t="s">
         <v>1</v>
@@ -8849,8 +8849,8 @@
       <c r="B72" s="15" t="s">
         <v>584</v>
       </c>
-      <c r="C72" s="126" t="s">
-        <v>32</v>
+      <c r="C72" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D72" s="17" t="s">
         <v>1</v>
@@ -8875,8 +8875,8 @@
       <c r="B73" s="15" t="s">
         <v>585</v>
       </c>
-      <c r="C73" s="126" t="s">
-        <v>32</v>
+      <c r="C73" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D73" s="17" t="s">
         <v>1</v>
@@ -8901,8 +8901,8 @@
       <c r="B74" s="15" t="s">
         <v>663</v>
       </c>
-      <c r="C74" s="126" t="s">
-        <v>32</v>
+      <c r="C74" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D74" s="17" t="s">
         <v>1</v>
@@ -8927,8 +8927,8 @@
       <c r="B75" s="37" t="s">
         <v>586</v>
       </c>
-      <c r="C75" s="126" t="s">
-        <v>32</v>
+      <c r="C75" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D75" s="17" t="s">
         <v>1</v>
@@ -8953,8 +8953,8 @@
       <c r="B76" s="15" t="s">
         <v>705</v>
       </c>
-      <c r="C76" s="126" t="s">
-        <v>32</v>
+      <c r="C76" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D76" s="17" t="s">
         <v>1</v>
@@ -8979,8 +8979,8 @@
       <c r="B77" s="37" t="s">
         <v>707</v>
       </c>
-      <c r="C77" s="126" t="s">
-        <v>32</v>
+      <c r="C77" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D77" s="17" t="s">
         <v>1</v>
@@ -9005,8 +9005,8 @@
       <c r="B78" s="37" t="s">
         <v>708</v>
       </c>
-      <c r="C78" s="126" t="s">
-        <v>32</v>
+      <c r="C78" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D78" s="17" t="s">
         <v>1</v>
@@ -9031,8 +9031,8 @@
       <c r="B79" s="37" t="s">
         <v>711</v>
       </c>
-      <c r="C79" s="126" t="s">
-        <v>32</v>
+      <c r="C79" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D79" s="17" t="s">
         <v>1</v>
@@ -9057,8 +9057,8 @@
       <c r="B80" s="37" t="s">
         <v>716</v>
       </c>
-      <c r="C80" s="126" t="s">
-        <v>32</v>
+      <c r="C80" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D80" s="17" t="s">
         <v>1</v>
@@ -9083,8 +9083,8 @@
       <c r="B81" s="37" t="s">
         <v>720</v>
       </c>
-      <c r="C81" s="126" t="s">
-        <v>32</v>
+      <c r="C81" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D81" s="17" t="s">
         <v>1</v>
@@ -9109,8 +9109,8 @@
       <c r="B82" s="37" t="s">
         <v>723</v>
       </c>
-      <c r="C82" s="126" t="s">
-        <v>32</v>
+      <c r="C82" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D82" s="17" t="s">
         <v>1</v>
@@ -9135,8 +9135,8 @@
       <c r="B83" s="37" t="s">
         <v>724</v>
       </c>
-      <c r="C83" s="126" t="s">
-        <v>32</v>
+      <c r="C83" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D83" s="17" t="s">
         <v>1</v>
@@ -9161,8 +9161,8 @@
       <c r="B84" s="37" t="s">
         <v>729</v>
       </c>
-      <c r="C84" s="126" t="s">
-        <v>32</v>
+      <c r="C84" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D84" s="17" t="s">
         <v>1</v>
@@ -9187,8 +9187,8 @@
       <c r="B85" s="37" t="s">
         <v>734</v>
       </c>
-      <c r="C85" s="126" t="s">
-        <v>32</v>
+      <c r="C85" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D85" s="17" t="s">
         <v>1</v>
@@ -9213,8 +9213,8 @@
       <c r="B86" s="37" t="s">
         <v>736</v>
       </c>
-      <c r="C86" s="126" t="s">
-        <v>32</v>
+      <c r="C86" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D86" s="17" t="s">
         <v>1</v>
@@ -9239,8 +9239,8 @@
       <c r="B87" s="37" t="s">
         <v>754</v>
       </c>
-      <c r="C87" s="126" t="s">
-        <v>32</v>
+      <c r="C87" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D87" s="17" t="s">
         <v>1</v>
@@ -9265,8 +9265,8 @@
       <c r="B88" s="37" t="s">
         <v>756</v>
       </c>
-      <c r="C88" s="126" t="s">
-        <v>32</v>
+      <c r="C88" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D88" s="17" t="s">
         <v>1</v>
@@ -9291,8 +9291,8 @@
       <c r="B89" s="37" t="s">
         <v>757</v>
       </c>
-      <c r="C89" s="126" t="s">
-        <v>32</v>
+      <c r="C89" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D89" s="17" t="s">
         <v>1</v>
@@ -9317,8 +9317,8 @@
       <c r="B90" s="37" t="s">
         <v>760</v>
       </c>
-      <c r="C90" s="126" t="s">
-        <v>32</v>
+      <c r="C90" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D90" s="17" t="s">
         <v>1</v>
@@ -9343,8 +9343,8 @@
       <c r="B91" s="37" t="s">
         <v>762</v>
       </c>
-      <c r="C91" s="126" t="s">
-        <v>32</v>
+      <c r="C91" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D91" s="17" t="s">
         <v>1</v>
@@ -9369,8 +9369,8 @@
       <c r="B92" s="37" t="s">
         <v>765</v>
       </c>
-      <c r="C92" s="126" t="s">
-        <v>32</v>
+      <c r="C92" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D92" s="17" t="s">
         <v>1</v>
@@ -9395,8 +9395,8 @@
       <c r="B93" s="37" t="s">
         <v>767</v>
       </c>
-      <c r="C93" s="126" t="s">
-        <v>32</v>
+      <c r="C93" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D93" s="17" t="s">
         <v>1</v>
@@ -9421,8 +9421,8 @@
       <c r="B94" s="37" t="s">
         <v>768</v>
       </c>
-      <c r="C94" s="126" t="s">
-        <v>32</v>
+      <c r="C94" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D94" s="17" t="s">
         <v>1</v>
@@ -9447,8 +9447,8 @@
       <c r="B95" s="37" t="s">
         <v>771</v>
       </c>
-      <c r="C95" s="126" t="s">
-        <v>32</v>
+      <c r="C95" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D95" s="17" t="s">
         <v>1</v>
@@ -9473,8 +9473,8 @@
       <c r="B96" s="37" t="s">
         <v>775</v>
       </c>
-      <c r="C96" s="126" t="s">
-        <v>32</v>
+      <c r="C96" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D96" s="17" t="s">
         <v>1</v>
@@ -9499,8 +9499,8 @@
       <c r="B97" s="41" t="s">
         <v>779</v>
       </c>
-      <c r="C97" s="126" t="s">
-        <v>32</v>
+      <c r="C97" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D97" s="17" t="s">
         <v>1</v>
@@ -9525,8 +9525,8 @@
       <c r="B98" s="37" t="s">
         <v>790</v>
       </c>
-      <c r="C98" s="126" t="s">
-        <v>32</v>
+      <c r="C98" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D98" s="17" t="s">
         <v>1</v>
@@ -9551,8 +9551,8 @@
       <c r="B99" s="37" t="s">
         <v>791</v>
       </c>
-      <c r="C99" s="126" t="s">
-        <v>32</v>
+      <c r="C99" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D99" s="17" t="s">
         <v>1</v>
@@ -9577,8 +9577,8 @@
       <c r="B100" s="37" t="s">
         <v>794</v>
       </c>
-      <c r="C100" s="126" t="s">
-        <v>32</v>
+      <c r="C100" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D100" s="17" t="s">
         <v>1</v>
@@ -9603,8 +9603,8 @@
       <c r="B101" s="37" t="s">
         <v>795</v>
       </c>
-      <c r="C101" s="126" t="s">
-        <v>32</v>
+      <c r="C101" s="145" t="s">
+        <v>33</v>
       </c>
       <c r="D101" s="17" t="s">
         <v>1</v>
@@ -9629,8 +9629,8 @@
       <c r="B102" s="37" t="s">
         <v>801</v>
       </c>
-      <c r="C102" s="126" t="s">
-        <v>32</v>
+      <c r="C102" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D102" s="17" t="s">
         <v>1</v>
@@ -9655,8 +9655,8 @@
       <c r="B103" s="37" t="s">
         <v>802</v>
       </c>
-      <c r="C103" s="126" t="s">
-        <v>32</v>
+      <c r="C103" s="132" t="s">
+        <v>33</v>
       </c>
       <c r="D103" s="17" t="s">
         <v>1</v>
@@ -9682,7 +9682,7 @@
         <v>818</v>
       </c>
       <c r="C104" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D104" s="17" t="s">
         <v>1</v>
@@ -9708,7 +9708,7 @@
         <v>819</v>
       </c>
       <c r="C105" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D105" s="17" t="s">
         <v>1</v>
@@ -9734,7 +9734,7 @@
         <v>820</v>
       </c>
       <c r="C106" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D106" s="17" t="s">
         <v>1</v>
@@ -9760,7 +9760,7 @@
         <v>817</v>
       </c>
       <c r="C107" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D107" s="17" t="s">
         <v>1</v>
@@ -9786,7 +9786,7 @@
         <v>827</v>
       </c>
       <c r="C108" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D108" s="17" t="s">
         <v>1</v>
@@ -9812,7 +9812,7 @@
         <v>830</v>
       </c>
       <c r="C109" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D109" s="17" t="s">
         <v>1</v>
@@ -9838,7 +9838,7 @@
         <v>833</v>
       </c>
       <c r="C110" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D110" s="17" t="s">
         <v>1</v>
@@ -9864,7 +9864,7 @@
         <v>834</v>
       </c>
       <c r="C111" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D111" s="17" t="s">
         <v>1</v>
@@ -9890,7 +9890,7 @@
         <v>842</v>
       </c>
       <c r="C112" s="146" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D112" s="17" t="s">
         <v>1</v>
@@ -9916,7 +9916,7 @@
         <v>847</v>
       </c>
       <c r="C113" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D113" s="17" t="s">
         <v>1</v>
@@ -9942,7 +9942,7 @@
         <v>853</v>
       </c>
       <c r="C114" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D114" s="17" t="s">
         <v>1</v>
@@ -9968,7 +9968,7 @@
         <v>854</v>
       </c>
       <c r="C115" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D115" s="17" t="s">
         <v>1</v>
@@ -9994,7 +9994,7 @@
         <v>858</v>
       </c>
       <c r="C116" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D116" s="17" t="s">
         <v>1</v>
@@ -10020,7 +10020,7 @@
         <v>861</v>
       </c>
       <c r="C117" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D117" s="17" t="s">
         <v>1</v>
@@ -10046,7 +10046,7 @@
         <v>867</v>
       </c>
       <c r="C118" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D118" s="17" t="s">
         <v>1</v>
@@ -10072,7 +10072,7 @@
         <v>868</v>
       </c>
       <c r="C119" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D119" s="17" t="s">
         <v>1</v>
@@ -10098,7 +10098,7 @@
         <v>871</v>
       </c>
       <c r="C120" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D120" s="97" t="s">
         <v>1</v>
@@ -10126,7 +10126,7 @@
         <v>876</v>
       </c>
       <c r="C121" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D121" s="17" t="s">
         <v>1</v>
@@ -10152,7 +10152,7 @@
         <v>880</v>
       </c>
       <c r="C122" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D122" s="17" t="s">
         <v>1</v>
@@ -10178,7 +10178,7 @@
         <v>893</v>
       </c>
       <c r="C123" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D123" s="17" t="s">
         <v>1</v>
@@ -10204,7 +10204,7 @@
         <v>876</v>
       </c>
       <c r="C124" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D124" s="26" t="s">
         <v>1</v>
@@ -10230,7 +10230,7 @@
         <v>899</v>
       </c>
       <c r="C125" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D125" s="26" t="s">
         <v>1</v>
@@ -10251,7 +10251,7 @@
         <v>900</v>
       </c>
       <c r="C126" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D126" s="26" t="s">
         <v>1</v>
@@ -10272,7 +10272,7 @@
         <v>901</v>
       </c>
       <c r="C127" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D127" s="26" t="s">
         <v>1</v>
@@ -10293,7 +10293,7 @@
         <v>902</v>
       </c>
       <c r="C128" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D128" s="26" t="s">
         <v>1</v>
@@ -10314,7 +10314,7 @@
         <v>903</v>
       </c>
       <c r="C129" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D129" s="26" t="s">
         <v>1</v>
@@ -10335,7 +10335,7 @@
         <v>904</v>
       </c>
       <c r="C130" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D130" s="26" t="s">
         <v>1</v>
@@ -10356,7 +10356,7 @@
         <v>905</v>
       </c>
       <c r="C131" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D131" s="26" t="s">
         <v>1</v>
@@ -10377,7 +10377,7 @@
         <v>28</v>
       </c>
       <c r="C132" s="146" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D132" s="19" t="s">
         <v>25</v>
@@ -10407,7 +10407,7 @@
         <v>456</v>
       </c>
       <c r="C133" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D133" s="19" t="s">
         <v>25</v>
@@ -10437,7 +10437,7 @@
         <v>460</v>
       </c>
       <c r="C134" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D134" s="19" t="s">
         <v>25</v>
@@ -10467,7 +10467,7 @@
         <v>445</v>
       </c>
       <c r="C135" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D135" s="19" t="s">
         <v>25</v>
@@ -10497,7 +10497,7 @@
         <v>89</v>
       </c>
       <c r="C136" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D136" s="19" t="s">
         <v>25</v>
@@ -10527,7 +10527,7 @@
         <v>94</v>
       </c>
       <c r="C137" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D137" s="19" t="s">
         <v>25</v>
@@ -10557,7 +10557,7 @@
         <v>98</v>
       </c>
       <c r="C138" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D138" s="19" t="s">
         <v>25</v>
@@ -10587,7 +10587,7 @@
         <v>103</v>
       </c>
       <c r="C139" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D139" s="19" t="s">
         <v>25</v>
@@ -10617,7 +10617,7 @@
         <v>106</v>
       </c>
       <c r="C140" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D140" s="19" t="s">
         <v>25</v>
@@ -10647,7 +10647,7 @@
         <v>109</v>
       </c>
       <c r="C141" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D141" s="19" t="s">
         <v>25</v>
@@ -10677,7 +10677,7 @@
         <v>112</v>
       </c>
       <c r="C142" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D142" s="19" t="s">
         <v>25</v>
@@ -10707,7 +10707,7 @@
         <v>119</v>
       </c>
       <c r="C143" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D143" s="19" t="s">
         <v>25</v>
@@ -10737,7 +10737,7 @@
         <v>126</v>
       </c>
       <c r="C144" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D144" s="19" t="s">
         <v>25</v>
@@ -10939,7 +10939,7 @@
         <v>462</v>
       </c>
       <c r="C151" s="133" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D151" s="19" t="s">
         <v>25</v>
@@ -11051,7 +11051,7 @@
         <v>582</v>
       </c>
       <c r="C155" s="133" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D155" s="17" t="s">
         <v>25</v>
@@ -11133,7 +11133,7 @@
         <v>589</v>
       </c>
       <c r="C158" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D158" s="19" t="s">
         <v>25</v>
@@ -11359,7 +11359,7 @@
         <v>886</v>
       </c>
       <c r="C166" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D166" s="19" t="s">
         <v>25</v>
@@ -11387,7 +11387,7 @@
         <v>886</v>
       </c>
       <c r="C167" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D167" s="19" t="s">
         <v>25</v>
@@ -11501,7 +11501,7 @@
         <v>413</v>
       </c>
       <c r="C171" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D171" s="27" t="s">
         <v>216</v>
@@ -11677,7 +11677,7 @@
         <v>418</v>
       </c>
       <c r="C177" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D177" s="26" t="s">
         <v>216</v>
@@ -11761,7 +11761,7 @@
         <v>949</v>
       </c>
       <c r="C180" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D180" s="100" t="s">
         <v>950</v>
@@ -11788,7 +11788,7 @@
         <v>952</v>
       </c>
       <c r="C181" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D181" s="100" t="s">
         <v>950</v>
@@ -11815,7 +11815,7 @@
         <v>954</v>
       </c>
       <c r="C182" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D182" s="100" t="s">
         <v>950</v>
@@ -11842,7 +11842,7 @@
         <v>957</v>
       </c>
       <c r="C183" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D183" s="100" t="s">
         <v>950</v>
@@ -11869,7 +11869,7 @@
         <v>959</v>
       </c>
       <c r="C184" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D184" s="100" t="s">
         <v>950</v>
@@ -11896,7 +11896,7 @@
         <v>960</v>
       </c>
       <c r="C185" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D185" s="100" t="s">
         <v>950</v>
@@ -11923,7 +11923,7 @@
         <v>961</v>
       </c>
       <c r="C186" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D186" s="100" t="s">
         <v>950</v>
@@ -11950,7 +11950,7 @@
         <v>962</v>
       </c>
       <c r="C187" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D187" s="100" t="s">
         <v>950</v>
@@ -11977,7 +11977,7 @@
         <v>963</v>
       </c>
       <c r="C188" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D188" s="100" t="s">
         <v>950</v>
@@ -12004,7 +12004,7 @@
         <v>964</v>
       </c>
       <c r="C189" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D189" s="100" t="s">
         <v>950</v>
@@ -12031,7 +12031,7 @@
         <v>965</v>
       </c>
       <c r="C190" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D190" s="100" t="s">
         <v>950</v>
@@ -12052,7 +12052,7 @@
         <v>966</v>
       </c>
       <c r="C191" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D191" s="100" t="s">
         <v>950</v>
@@ -12073,7 +12073,7 @@
         <v>967</v>
       </c>
       <c r="C192" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D192" s="100" t="s">
         <v>950</v>
@@ -12094,7 +12094,7 @@
         <v>968</v>
       </c>
       <c r="C193" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D193" s="100" t="s">
         <v>950</v>
@@ -12115,7 +12115,7 @@
         <v>969</v>
       </c>
       <c r="C194" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D194" s="100" t="s">
         <v>950</v>
@@ -12136,7 +12136,7 @@
         <v>970</v>
       </c>
       <c r="C195" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D195" s="100" t="s">
         <v>950</v>
@@ -12157,7 +12157,7 @@
         <v>971</v>
       </c>
       <c r="C196" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D196" s="100" t="s">
         <v>950</v>
@@ -12178,7 +12178,7 @@
         <v>973</v>
       </c>
       <c r="C197" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D197" s="100" t="s">
         <v>950</v>
@@ -12199,7 +12199,7 @@
         <v>975</v>
       </c>
       <c r="C198" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D198" s="100" t="s">
         <v>950</v>
@@ -12220,7 +12220,7 @@
         <v>976</v>
       </c>
       <c r="C199" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D199" s="100" t="s">
         <v>950</v>
@@ -12241,7 +12241,7 @@
         <v>978</v>
       </c>
       <c r="C200" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D200" s="100" t="s">
         <v>950</v>
@@ -12262,7 +12262,7 @@
         <v>979</v>
       </c>
       <c r="C201" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D201" s="100" t="s">
         <v>950</v>
@@ -12283,7 +12283,7 @@
         <v>980</v>
       </c>
       <c r="C202" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D202" s="100" t="s">
         <v>981</v>
@@ -12310,7 +12310,7 @@
         <v>983</v>
       </c>
       <c r="C203" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D203" s="100" t="s">
         <v>981</v>
@@ -12337,7 +12337,7 @@
         <v>985</v>
       </c>
       <c r="C204" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D204" s="100" t="s">
         <v>981</v>
@@ -12364,7 +12364,7 @@
         <v>986</v>
       </c>
       <c r="C205" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D205" s="100" t="s">
         <v>981</v>
@@ -12391,7 +12391,7 @@
         <v>989</v>
       </c>
       <c r="C206" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D206" s="109" t="s">
         <v>981</v>
@@ -12421,7 +12421,7 @@
         <v>991</v>
       </c>
       <c r="C207" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D207" s="109" t="s">
         <v>981</v>
@@ -12447,7 +12447,7 @@
         <v>993</v>
       </c>
       <c r="C208" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D208" s="109" t="s">
         <v>981</v>
@@ -12470,7 +12470,7 @@
         <v>995</v>
       </c>
       <c r="C209" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D209" s="109" t="s">
         <v>981</v>
@@ -12496,7 +12496,7 @@
         <v>997</v>
       </c>
       <c r="C210" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D210" s="109" t="s">
         <v>981</v>
@@ -12522,7 +12522,7 @@
         <v>1001</v>
       </c>
       <c r="C211" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D211" s="109" t="s">
         <v>981</v>
@@ -12548,7 +12548,7 @@
         <v>948</v>
       </c>
       <c r="C212" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D212" s="109" t="s">
         <v>1003</v>
@@ -12574,7 +12574,7 @@
         <v>1004</v>
       </c>
       <c r="C213" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D213" s="109" t="s">
         <v>1003</v>
@@ -12594,7 +12594,7 @@
         <v>1005</v>
       </c>
       <c r="C214" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D214" s="109" t="s">
         <v>1003</v>
@@ -12614,7 +12614,7 @@
         <v>1036</v>
       </c>
       <c r="C215" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D215" s="109" t="s">
         <v>1003</v>
@@ -12634,7 +12634,7 @@
         <v>1041</v>
       </c>
       <c r="C216" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D216" s="109" t="s">
         <v>1003</v>
@@ -12654,7 +12654,7 @@
         <v>995</v>
       </c>
       <c r="C217" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D217" s="109" t="s">
         <v>1003</v>
@@ -12674,7 +12674,7 @@
         <v>440</v>
       </c>
       <c r="C218" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D218" s="109" t="s">
         <v>1014</v>
@@ -12700,7 +12700,7 @@
         <v>1006</v>
       </c>
       <c r="C219" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D219" s="109" t="s">
         <v>1014</v>
@@ -12723,7 +12723,7 @@
         <v>1008</v>
       </c>
       <c r="C220" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D220" s="109" t="s">
         <v>1014</v>
@@ -12746,7 +12746,7 @@
         <v>1010</v>
       </c>
       <c r="C221" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D221" s="109" t="s">
         <v>1014</v>
@@ -12769,7 +12769,7 @@
         <v>1012</v>
       </c>
       <c r="C222" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D222" s="109" t="s">
         <v>1014</v>
@@ -12792,7 +12792,7 @@
         <v>1018</v>
       </c>
       <c r="C223" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D223" s="109" t="s">
         <v>1014</v>
@@ -12815,7 +12815,7 @@
         <v>1015</v>
       </c>
       <c r="C224" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D224" s="109" t="s">
         <v>1014</v>
@@ -12838,7 +12838,7 @@
         <v>1020</v>
       </c>
       <c r="C225" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D225" s="109" t="s">
         <v>1014</v>
@@ -12858,7 +12858,7 @@
         <v>1024</v>
       </c>
       <c r="C226" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D226" s="109" t="s">
         <v>1014</v>
@@ -12878,7 +12878,7 @@
         <v>1026</v>
       </c>
       <c r="C227" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D227" s="109" t="s">
         <v>1014</v>
@@ -12898,7 +12898,7 @@
         <v>1028</v>
       </c>
       <c r="C228" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D228" s="109" t="s">
         <v>1014</v>
@@ -12918,7 +12918,7 @@
         <v>1030</v>
       </c>
       <c r="C229" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D229" s="100" t="s">
         <v>396</v>
@@ -12941,7 +12941,7 @@
         <v>1031</v>
       </c>
       <c r="C230" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D230" s="100" t="s">
         <v>396</v>
@@ -12964,7 +12964,7 @@
         <v>1034</v>
       </c>
       <c r="C231" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D231" s="100" t="s">
         <v>396</v>
@@ -12987,7 +12987,7 @@
         <v>1060</v>
       </c>
       <c r="C232" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D232" s="100" t="s">
         <v>1062</v>
@@ -13007,7 +13007,7 @@
         <v>1063</v>
       </c>
       <c r="C233" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D233" s="100" t="s">
         <v>1062</v>
@@ -13027,7 +13027,7 @@
         <v>1065</v>
       </c>
       <c r="C234" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D234" s="100" t="s">
         <v>1062</v>
@@ -13047,7 +13047,7 @@
         <v>1066</v>
       </c>
       <c r="C235" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D235" s="100" t="s">
         <v>1062</v>
@@ -13067,7 +13067,7 @@
         <v>1067</v>
       </c>
       <c r="C236" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D236" s="100" t="s">
         <v>1062</v>
@@ -13087,7 +13087,7 @@
         <v>1071</v>
       </c>
       <c r="C237" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D237" s="100" t="s">
         <v>1062</v>
@@ -13107,7 +13107,7 @@
         <v>1073</v>
       </c>
       <c r="C238" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D238" s="100" t="s">
         <v>1075</v>
@@ -13127,7 +13127,7 @@
         <v>1077</v>
       </c>
       <c r="C239" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D239" s="100" t="s">
         <v>1075</v>
@@ -13147,7 +13147,7 @@
         <v>540</v>
       </c>
       <c r="C240" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D240" s="100" t="s">
         <v>1075</v>
@@ -13173,7 +13173,7 @@
         <v>60</v>
       </c>
       <c r="C241" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D241" s="100" t="s">
         <v>1075</v>
@@ -13199,7 +13199,7 @@
         <v>906</v>
       </c>
       <c r="C242" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D242" s="26" t="s">
         <v>1075</v>
@@ -13220,7 +13220,7 @@
         <v>373</v>
       </c>
       <c r="C243" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D243" s="17" t="s">
         <v>1079</v>
@@ -13246,7 +13246,7 @@
         <v>356</v>
       </c>
       <c r="C244" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D244" s="17" t="s">
         <v>1079</v>
@@ -13272,7 +13272,7 @@
         <v>1044</v>
       </c>
       <c r="C245" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D245" s="17" t="s">
         <v>1079</v>
@@ -13292,7 +13292,7 @@
         <v>1054</v>
       </c>
       <c r="C246" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D246" s="17" t="s">
         <v>1079</v>
@@ -13312,7 +13312,7 @@
         <v>1056</v>
       </c>
       <c r="C247" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D247" s="17" t="s">
         <v>1079</v>
@@ -13332,7 +13332,7 @@
         <v>1058</v>
       </c>
       <c r="C248" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D248" s="17" t="s">
         <v>1079</v>
@@ -13352,7 +13352,7 @@
         <v>341</v>
       </c>
       <c r="C249" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D249" s="17" t="s">
         <v>1079</v>
@@ -13380,7 +13380,7 @@
         <v>340</v>
       </c>
       <c r="C250" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D250" s="17" t="s">
         <v>1079</v>
@@ -13408,7 +13408,7 @@
         <v>1080</v>
       </c>
       <c r="C251" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D251" s="126" t="s">
         <v>1081</v>
@@ -13431,7 +13431,7 @@
         <v>1093</v>
       </c>
       <c r="C252" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D252" s="126" t="s">
         <v>1081</v>
@@ -13454,7 +13454,7 @@
         <v>1094</v>
       </c>
       <c r="C253" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D253" s="126" t="s">
         <v>1081</v>
@@ -13477,7 +13477,7 @@
         <v>1096</v>
       </c>
       <c r="C254" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D254" s="126" t="s">
         <v>1081</v>
@@ -13500,7 +13500,7 @@
         <v>1105</v>
       </c>
       <c r="C255" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D255" s="126" t="s">
         <v>1081</v>
@@ -13520,7 +13520,7 @@
         <v>1107</v>
       </c>
       <c r="C256" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D256" s="126" t="s">
         <v>1081</v>
@@ -13543,7 +13543,7 @@
         <v>1118</v>
       </c>
       <c r="C257" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D257" s="126" t="s">
         <v>1081</v>
@@ -13566,7 +13566,7 @@
         <v>1119</v>
       </c>
       <c r="C258" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D258" s="126" t="s">
         <v>1081</v>
@@ -13589,7 +13589,7 @@
         <v>1120</v>
       </c>
       <c r="C259" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D259" s="126" t="s">
         <v>1081</v>
@@ -13612,7 +13612,7 @@
         <v>1134</v>
       </c>
       <c r="C260" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D260" s="126" t="s">
         <v>1081</v>
@@ -13638,7 +13638,7 @@
         <v>1132</v>
       </c>
       <c r="C261" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D261" s="126" t="s">
         <v>1081</v>
@@ -13664,7 +13664,7 @@
         <v>1133</v>
       </c>
       <c r="C262" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D262" s="126" t="s">
         <v>1081</v>
@@ -13690,7 +13690,7 @@
         <v>1144</v>
       </c>
       <c r="C263" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D263" s="126" t="s">
         <v>1081</v>
@@ -13716,7 +13716,7 @@
         <v>1194</v>
       </c>
       <c r="C264" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D264" s="126" t="s">
         <v>1081</v>
@@ -13742,7 +13742,7 @@
         <v>1200</v>
       </c>
       <c r="C265" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D265" s="126" t="s">
         <v>1081</v>
@@ -13768,7 +13768,7 @@
         <v>1204</v>
       </c>
       <c r="C266" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D266" s="126" t="s">
         <v>1081</v>
@@ -13794,7 +13794,7 @@
         <v>1209</v>
       </c>
       <c r="C267" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D267" s="126" t="s">
         <v>1211</v>
@@ -13817,7 +13817,7 @@
         <v>1215</v>
       </c>
       <c r="C268" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D268" s="126" t="s">
         <v>1211</v>
@@ -13840,7 +13840,7 @@
         <v>1217</v>
       </c>
       <c r="C269" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D269" s="126" t="s">
         <v>1211</v>
@@ -13863,7 +13863,7 @@
         <v>1246</v>
       </c>
       <c r="C270" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D270" s="126" t="s">
         <v>1211</v>
@@ -13886,7 +13886,7 @@
         <v>1218</v>
       </c>
       <c r="C271" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D271" s="126" t="s">
         <v>1219</v>
@@ -13909,7 +13909,7 @@
         <v>1230</v>
       </c>
       <c r="C272" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D272" s="126" t="s">
         <v>1219</v>
@@ -13932,7 +13932,7 @@
         <v>1234</v>
       </c>
       <c r="C273" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D273" s="126" t="s">
         <v>1219</v>
@@ -13955,7 +13955,7 @@
         <v>1240</v>
       </c>
       <c r="C274" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D274" s="126" t="s">
         <v>1219</v>
@@ -13978,7 +13978,7 @@
         <v>1248</v>
       </c>
       <c r="C275" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D275" s="126" t="s">
         <v>1219</v>
@@ -14001,7 +14001,7 @@
         <v>1252</v>
       </c>
       <c r="C276" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D276" s="126" t="s">
         <v>1219</v>
@@ -14024,7 +14024,7 @@
         <v>1254</v>
       </c>
       <c r="C277" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D277" s="126" t="s">
         <v>1219</v>
@@ -14047,7 +14047,7 @@
         <v>1268</v>
       </c>
       <c r="C278" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D278" s="126" t="s">
         <v>1219</v>
@@ -14070,7 +14070,7 @@
         <v>1269</v>
       </c>
       <c r="C279" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D279" s="126" t="s">
         <v>1219</v>
@@ -14093,7 +14093,7 @@
         <v>1257</v>
       </c>
       <c r="C280" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D280" s="126" t="s">
         <v>1256</v>
@@ -14116,7 +14116,7 @@
         <v>1267</v>
       </c>
       <c r="C281" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D281" s="126" t="s">
         <v>1256</v>
@@ -14139,7 +14139,7 @@
         <v>1273</v>
       </c>
       <c r="C282" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D282" s="126" t="s">
         <v>1282</v>
@@ -14162,7 +14162,7 @@
         <v>1286</v>
       </c>
       <c r="C283" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D283" s="126" t="s">
         <v>1282</v>
@@ -14185,7 +14185,7 @@
         <v>1321</v>
       </c>
       <c r="C284" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D284" s="126" t="s">
         <v>1282</v>
@@ -14208,7 +14208,7 @@
         <v>1285</v>
       </c>
       <c r="C285" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D285" s="128" t="s">
         <v>1284</v>
@@ -14231,7 +14231,7 @@
         <v>1289</v>
       </c>
       <c r="C286" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D286" s="128" t="s">
         <v>1284</v>
@@ -14254,7 +14254,7 @@
         <v>1291</v>
       </c>
       <c r="C287" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D287" s="128" t="s">
         <v>1284</v>
@@ -14277,7 +14277,7 @@
         <v>1294</v>
       </c>
       <c r="C288" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D288" s="128" t="s">
         <v>1293</v>
@@ -14300,7 +14300,7 @@
         <v>1306</v>
       </c>
       <c r="C289" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D289" s="128" t="s">
         <v>1293</v>
@@ -14323,7 +14323,7 @@
         <v>1421</v>
       </c>
       <c r="C290" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D290" s="128" t="s">
         <v>1293</v>
@@ -14346,7 +14346,7 @@
         <v>1353</v>
       </c>
       <c r="C291" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D291" s="128" t="s">
         <v>1293</v>
@@ -14369,7 +14369,7 @@
         <v>1330</v>
       </c>
       <c r="C292" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D292" s="17" t="s">
         <v>1</v>
@@ -14392,7 +14392,7 @@
         <v>1332</v>
       </c>
       <c r="C293" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D293" s="17" t="s">
         <v>1</v>
@@ -14418,7 +14418,7 @@
         <v>1334</v>
       </c>
       <c r="C294" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D294" s="17" t="s">
         <v>1</v>
@@ -14444,7 +14444,7 @@
         <v>1338</v>
       </c>
       <c r="C295" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D295" s="19" t="s">
         <v>25</v>
@@ -14467,7 +14467,7 @@
         <v>1340</v>
       </c>
       <c r="C296" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D296" s="17" t="s">
         <v>1</v>
@@ -14487,7 +14487,7 @@
         <v>1341</v>
       </c>
       <c r="C297" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D297" s="17" t="s">
         <v>1</v>
@@ -14510,7 +14510,7 @@
         <v>1351</v>
       </c>
       <c r="C298" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D298" s="17" t="s">
         <v>1</v>
@@ -14533,7 +14533,7 @@
         <v>1353</v>
       </c>
       <c r="C299" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D299" s="17" t="s">
         <v>1</v>
@@ -14556,7 +14556,7 @@
         <v>1357</v>
       </c>
       <c r="C300" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D300" s="17" t="s">
         <v>1</v>
@@ -14579,7 +14579,7 @@
         <v>1363</v>
       </c>
       <c r="C301" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D301" s="17" t="s">
         <v>981</v>
@@ -14599,7 +14599,7 @@
         <v>1364</v>
       </c>
       <c r="C302" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D302" s="17" t="s">
         <v>1</v>
@@ -14622,7 +14622,7 @@
         <v>1365</v>
       </c>
       <c r="C303" s="137" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D303" s="19" t="s">
         <v>25</v>
@@ -14645,7 +14645,7 @@
         <v>1369</v>
       </c>
       <c r="C304" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D304" s="126" t="s">
         <v>1368</v>
@@ -14671,7 +14671,7 @@
         <v>1373</v>
       </c>
       <c r="C305" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D305" s="126" t="s">
         <v>1368</v>
@@ -14694,7 +14694,7 @@
         <v>1377</v>
       </c>
       <c r="C306" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D306" s="126" t="s">
         <v>1368</v>
@@ -14717,7 +14717,7 @@
         <v>1381</v>
       </c>
       <c r="C307" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D307" s="126" t="s">
         <v>1368</v>
@@ -14740,7 +14740,7 @@
         <v>1385</v>
       </c>
       <c r="C308" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D308" s="126" t="s">
         <v>1368</v>
@@ -14766,7 +14766,7 @@
         <v>1386</v>
       </c>
       <c r="C309" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D309" s="126" t="s">
         <v>1368</v>
@@ -14792,7 +14792,7 @@
         <v>1390</v>
       </c>
       <c r="C310" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D310" s="126" t="s">
         <v>1368</v>
@@ -14818,7 +14818,7 @@
         <v>1392</v>
       </c>
       <c r="C311" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D311" s="126" t="s">
         <v>1368</v>
@@ -14844,7 +14844,7 @@
         <v>1400</v>
       </c>
       <c r="C312" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D312" s="126" t="s">
         <v>1368</v>
@@ -14870,7 +14870,7 @@
         <v>1407</v>
       </c>
       <c r="C313" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D313" s="126" t="s">
         <v>1368</v>
@@ -14896,7 +14896,7 @@
         <v>1412</v>
       </c>
       <c r="C314" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D314" s="126" t="s">
         <v>1368</v>
@@ -14922,7 +14922,7 @@
         <v>1416</v>
       </c>
       <c r="C315" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D315" s="126" t="s">
         <v>1368</v>
@@ -14948,7 +14948,7 @@
         <v>1426</v>
       </c>
       <c r="C316" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D316" s="126" t="s">
         <v>1</v>
@@ -14974,7 +14974,7 @@
         <v>1434</v>
       </c>
       <c r="C317" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D317" s="126" t="s">
         <v>1</v>
@@ -15000,7 +15000,7 @@
         <v>1440</v>
       </c>
       <c r="C318" s="126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D318" s="126" t="s">
         <v>1</v>
@@ -29482,7 +29482,7 @@
   <dimension ref="A1:FY13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39343,7 +39343,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39630,7 +39630,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Wave 1 2023 Part 3 Run Cloud Stage
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics_CRM_Cloud_2023_Wave1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F68E06-7385-4707-BDE6-A3A9FD936CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD87FCD-EFCB-44B0-AE8C-35C92003980D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -6779,10 +6779,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6835,7 +6836,7 @@
       </c>
       <c r="L1" s="104"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -6869,7 +6870,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>2</v>
       </c>
@@ -6901,7 +6902,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -6931,7 +6932,7 @@
       <c r="K4" s="17"/>
       <c r="L4" s="105"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -6961,7 +6962,7 @@
       <c r="K5" s="17"/>
       <c r="L5" s="103"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>5</v>
       </c>
@@ -6989,7 +6990,7 @@
       <c r="K6" s="17"/>
       <c r="L6" s="105"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>6</v>
       </c>
@@ -7019,7 +7020,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>7</v>
       </c>
@@ -7051,7 +7052,7 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -7079,7 +7080,7 @@
       <c r="K9" s="17"/>
       <c r="L9" s="103"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>9</v>
       </c>
@@ -7109,7 +7110,7 @@
       <c r="K10" s="17"/>
       <c r="L10" s="103"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>10</v>
       </c>
@@ -7139,7 +7140,7 @@
       <c r="K11" s="17"/>
       <c r="L11" s="103"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>11</v>
       </c>
@@ -7170,7 +7171,7 @@
       <c r="L12" s="103"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>12</v>
       </c>
@@ -7198,7 +7199,7 @@
       <c r="K13" s="17"/>
       <c r="L13" s="103"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>13</v>
       </c>
@@ -7226,7 +7227,7 @@
       <c r="K14" s="17"/>
       <c r="L14" s="103"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>14</v>
       </c>
@@ -7256,7 +7257,7 @@
       <c r="K15" s="17"/>
       <c r="L15" s="103"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>15</v>
       </c>
@@ -7286,7 +7287,7 @@
       <c r="K16" s="17"/>
       <c r="L16" s="103"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>16</v>
       </c>
@@ -7314,7 +7315,7 @@
       <c r="K17" s="17"/>
       <c r="L17" s="103"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>17</v>
       </c>
@@ -7342,7 +7343,7 @@
       <c r="K18" s="17"/>
       <c r="L18" s="103"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>18</v>
       </c>
@@ -7368,7 +7369,7 @@
       <c r="K19" s="17"/>
       <c r="L19" s="103"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>19</v>
       </c>
@@ -7394,7 +7395,7 @@
       <c r="K20" s="23"/>
       <c r="L20" s="103"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>20</v>
       </c>
@@ -7424,7 +7425,7 @@
       <c r="K21" s="17"/>
       <c r="L21" s="103"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>21</v>
       </c>
@@ -7454,7 +7455,7 @@
       <c r="K22" s="17"/>
       <c r="L22" s="103"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>22</v>
       </c>
@@ -7484,7 +7485,7 @@
       <c r="K23" s="17"/>
       <c r="L23" s="103"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>23</v>
       </c>
@@ -7514,7 +7515,7 @@
       <c r="K24" s="17"/>
       <c r="L24" s="103"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>24</v>
       </c>
@@ -7544,7 +7545,7 @@
       <c r="K25" s="17"/>
       <c r="L25" s="103"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>25</v>
       </c>
@@ -7574,7 +7575,7 @@
       <c r="K26" s="17"/>
       <c r="L26" s="103"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>26</v>
       </c>
@@ -7602,7 +7603,7 @@
       <c r="K27" s="17"/>
       <c r="L27" s="103"/>
     </row>
-    <row r="28" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>27</v>
       </c>
@@ -7630,7 +7631,7 @@
       <c r="K28" s="17"/>
       <c r="L28" s="106"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>28</v>
       </c>
@@ -7658,7 +7659,7 @@
       <c r="K29" s="22"/>
       <c r="L29" s="103"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>29</v>
       </c>
@@ -7688,7 +7689,7 @@
       <c r="K30" s="22"/>
       <c r="L30" s="103"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>30</v>
       </c>
@@ -7716,7 +7717,7 @@
       <c r="K31" s="22"/>
       <c r="L31" s="103"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>31</v>
       </c>
@@ -7744,7 +7745,7 @@
       <c r="K32" s="22"/>
       <c r="L32" s="103"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>32</v>
       </c>
@@ -7772,7 +7773,7 @@
       <c r="K33" s="22"/>
       <c r="L33" s="103"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>33</v>
       </c>
@@ -7800,7 +7801,7 @@
       <c r="K34" s="22"/>
       <c r="L34" s="103"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>34</v>
       </c>
@@ -7828,7 +7829,7 @@
       <c r="K35" s="22"/>
       <c r="L35" s="103"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>35</v>
       </c>
@@ -7856,7 +7857,7 @@
       <c r="K36" s="22"/>
       <c r="L36" s="103"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>36</v>
       </c>
@@ -7884,7 +7885,7 @@
       <c r="K37" s="22"/>
       <c r="L37" s="103"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>37</v>
       </c>
@@ -7912,7 +7913,7 @@
       <c r="K38" s="22"/>
       <c r="L38" s="103"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>38</v>
       </c>
@@ -7940,7 +7941,7 @@
       <c r="K39" s="22"/>
       <c r="L39" s="103"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>39</v>
       </c>
@@ -7968,7 +7969,7 @@
       <c r="K40" s="22"/>
       <c r="L40" s="103"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>40</v>
       </c>
@@ -7996,7 +7997,7 @@
       <c r="K41" s="22"/>
       <c r="L41" s="103"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>41</v>
       </c>
@@ -8024,7 +8025,7 @@
       <c r="K42" s="22"/>
       <c r="L42" s="103"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>42</v>
       </c>
@@ -8052,7 +8053,7 @@
       <c r="K43" s="22"/>
       <c r="L43" s="103"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>43</v>
       </c>
@@ -8080,7 +8081,7 @@
       <c r="K44" s="22"/>
       <c r="L44" s="103"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>44</v>
       </c>
@@ -8108,7 +8109,7 @@
       <c r="K45" s="22"/>
       <c r="L45" s="103"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <v>45</v>
       </c>
@@ -8136,7 +8137,7 @@
       <c r="K46" s="22"/>
       <c r="L46" s="103"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>46</v>
       </c>
@@ -8164,7 +8165,7 @@
       <c r="K47" s="22"/>
       <c r="L47" s="103"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>47</v>
       </c>
@@ -8192,7 +8193,7 @@
       <c r="K48" s="22"/>
       <c r="L48" s="103"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>48</v>
       </c>
@@ -8220,7 +8221,7 @@
       <c r="K49" s="22"/>
       <c r="L49" s="103"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>49</v>
       </c>
@@ -8248,7 +8249,7 @@
       <c r="K50" s="22"/>
       <c r="L50" s="103"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>50</v>
       </c>
@@ -8276,7 +8277,7 @@
       <c r="K51" s="22"/>
       <c r="L51" s="103"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>51</v>
       </c>
@@ -8304,7 +8305,7 @@
       <c r="K52" s="22"/>
       <c r="L52" s="103"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
         <v>52</v>
       </c>
@@ -8332,7 +8333,7 @@
       <c r="K53" s="22"/>
       <c r="L53" s="103"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>53</v>
       </c>
@@ -8360,7 +8361,7 @@
       <c r="K54" s="22"/>
       <c r="L54" s="103"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
         <v>54</v>
       </c>
@@ -8388,7 +8389,7 @@
       <c r="K55" s="22"/>
       <c r="L55" s="103"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>55</v>
       </c>
@@ -8816,7 +8817,7 @@
       <c r="K70" s="22"/>
       <c r="L70" s="103"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
         <v>70</v>
       </c>
@@ -8842,7 +8843,7 @@
       <c r="K71" s="22"/>
       <c r="L71" s="103"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <v>71</v>
       </c>
@@ -8868,7 +8869,7 @@
       <c r="K72" s="22"/>
       <c r="L72" s="103"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>72</v>
       </c>
@@ -8894,7 +8895,7 @@
       <c r="K73" s="22"/>
       <c r="L73" s="103"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <v>73</v>
       </c>
@@ -8920,7 +8921,7 @@
       <c r="K74" s="22"/>
       <c r="L74" s="103"/>
     </row>
-    <row r="75" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <v>74</v>
       </c>
@@ -8946,7 +8947,7 @@
       <c r="K75" s="17"/>
       <c r="L75" s="106"/>
     </row>
-    <row r="76" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
         <v>75</v>
       </c>
@@ -8972,7 +8973,7 @@
       <c r="K76" s="17"/>
       <c r="L76" s="106"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="17">
         <v>76</v>
       </c>
@@ -8998,7 +8999,7 @@
       <c r="K77" s="45"/>
       <c r="L77" s="107"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <v>77</v>
       </c>
@@ -9024,7 +9025,7 @@
       <c r="K78" s="45"/>
       <c r="L78" s="107"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <v>78</v>
       </c>
@@ -9050,7 +9051,7 @@
       <c r="K79" s="45"/>
       <c r="L79" s="107"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <v>79</v>
       </c>
@@ -9076,7 +9077,7 @@
       <c r="K80" s="45"/>
       <c r="L80" s="107"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="17">
         <v>80</v>
       </c>
@@ -9102,7 +9103,7 @@
       <c r="K81" s="45"/>
       <c r="L81" s="107"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>81</v>
       </c>
@@ -9128,7 +9129,7 @@
       <c r="K82" s="45"/>
       <c r="L82" s="107"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>82</v>
       </c>
@@ -9154,7 +9155,7 @@
       <c r="K83" s="45"/>
       <c r="L83" s="107"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>83</v>
       </c>
@@ -9180,7 +9181,7 @@
       <c r="K84" s="45"/>
       <c r="L84" s="107"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>84</v>
       </c>
@@ -9206,7 +9207,7 @@
       <c r="K85" s="45"/>
       <c r="L85" s="107"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
         <v>85</v>
       </c>
@@ -9232,7 +9233,7 @@
       <c r="K86" s="45"/>
       <c r="L86" s="107"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="17">
         <v>86</v>
       </c>
@@ -9258,7 +9259,7 @@
       <c r="K87" s="45"/>
       <c r="L87" s="107"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
         <v>87</v>
       </c>
@@ -9284,7 +9285,7 @@
       <c r="K88" s="45"/>
       <c r="L88" s="107"/>
     </row>
-    <row r="89" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
         <v>88</v>
       </c>
@@ -9310,7 +9311,7 @@
       <c r="K89" s="17"/>
       <c r="L89" s="106"/>
     </row>
-    <row r="90" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="17">
         <v>89</v>
       </c>
@@ -9336,7 +9337,7 @@
       <c r="K90" s="17"/>
       <c r="L90" s="106"/>
     </row>
-    <row r="91" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="17">
         <v>90</v>
       </c>
@@ -9362,7 +9363,7 @@
       <c r="K91" s="17"/>
       <c r="L91" s="106"/>
     </row>
-    <row r="92" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
         <v>91</v>
       </c>
@@ -9388,7 +9389,7 @@
       <c r="K92" s="17"/>
       <c r="L92" s="106"/>
     </row>
-    <row r="93" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="17">
         <v>92</v>
       </c>
@@ -9414,7 +9415,7 @@
       <c r="K93" s="17"/>
       <c r="L93" s="106"/>
     </row>
-    <row r="94" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="17">
         <v>93</v>
       </c>
@@ -9440,7 +9441,7 @@
       <c r="K94" s="17"/>
       <c r="L94" s="106"/>
     </row>
-    <row r="95" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="17">
         <v>94</v>
       </c>
@@ -9466,7 +9467,7 @@
       <c r="K95" s="17"/>
       <c r="L95" s="106"/>
     </row>
-    <row r="96" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="17">
         <v>95</v>
       </c>
@@ -9492,7 +9493,7 @@
       <c r="K96" s="17"/>
       <c r="L96" s="106"/>
     </row>
-    <row r="97" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="17">
         <v>96</v>
       </c>
@@ -9518,7 +9519,7 @@
       <c r="K97" s="17"/>
       <c r="L97" s="106"/>
     </row>
-    <row r="98" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="17">
         <v>97</v>
       </c>
@@ -9544,7 +9545,7 @@
       <c r="K98" s="17"/>
       <c r="L98" s="106"/>
     </row>
-    <row r="99" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="17">
         <v>98</v>
       </c>
@@ -9570,7 +9571,7 @@
       <c r="K99" s="17"/>
       <c r="L99" s="106"/>
     </row>
-    <row r="100" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="17">
         <v>99</v>
       </c>
@@ -9596,7 +9597,7 @@
       <c r="K100" s="17"/>
       <c r="L100" s="106"/>
     </row>
-    <row r="101" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="17">
         <v>100</v>
       </c>
@@ -9622,7 +9623,7 @@
       <c r="K101" s="17"/>
       <c r="L101" s="106"/>
     </row>
-    <row r="102" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="17">
         <v>101</v>
       </c>
@@ -9648,7 +9649,7 @@
       <c r="K102" s="17"/>
       <c r="L102" s="106"/>
     </row>
-    <row r="103" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="17">
         <v>102</v>
       </c>
@@ -10759,7 +10760,7 @@
       <c r="K144" s="20"/>
       <c r="L144" s="103"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="17">
         <v>144</v>
       </c>
@@ -10787,7 +10788,7 @@
       <c r="K145" s="20"/>
       <c r="L145" s="103"/>
     </row>
-    <row r="146" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="17">
         <v>145</v>
       </c>
@@ -10817,7 +10818,7 @@
       <c r="K146" s="20"/>
       <c r="L146" s="106"/>
     </row>
-    <row r="147" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="17">
         <v>146</v>
       </c>
@@ -10847,7 +10848,7 @@
       <c r="K147" s="20"/>
       <c r="L147" s="106"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="17">
         <v>147</v>
       </c>
@@ -10875,7 +10876,7 @@
       <c r="K148" s="22"/>
       <c r="L148" s="103"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="17">
         <v>148</v>
       </c>
@@ -10903,7 +10904,7 @@
       <c r="K149" s="22"/>
       <c r="L149" s="103"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="17">
         <v>149</v>
       </c>
@@ -10959,7 +10960,7 @@
       <c r="K151" s="22"/>
       <c r="L151" s="103"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="17">
         <v>151</v>
       </c>
@@ -10987,7 +10988,7 @@
       <c r="K152" s="22"/>
       <c r="L152" s="103"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="17">
         <v>152</v>
       </c>
@@ -11015,7 +11016,7 @@
       <c r="K153" s="22"/>
       <c r="L153" s="103"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="17">
         <v>153</v>
       </c>
@@ -11069,7 +11070,7 @@
       <c r="K155" s="13"/>
       <c r="L155" s="103"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="17">
         <v>155</v>
       </c>
@@ -11097,7 +11098,7 @@
       <c r="K156" s="22"/>
       <c r="L156" s="103"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="17">
         <v>156</v>
       </c>
@@ -11155,7 +11156,7 @@
       <c r="K158" s="22"/>
       <c r="L158" s="103"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="17">
         <v>158</v>
       </c>
@@ -11183,7 +11184,7 @@
       <c r="K159" s="20"/>
       <c r="L159" s="103"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="17">
         <v>159</v>
       </c>
@@ -11211,7 +11212,7 @@
       <c r="K160" s="20"/>
       <c r="L160" s="103"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="17">
         <v>160</v>
       </c>
@@ -11239,7 +11240,7 @@
       <c r="K161" s="20"/>
       <c r="L161" s="103"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="17">
         <v>161</v>
       </c>
@@ -11267,7 +11268,7 @@
       <c r="K162" s="20"/>
       <c r="L162" s="103"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="17">
         <v>162</v>
       </c>
@@ -11295,7 +11296,7 @@
       <c r="K163" s="20"/>
       <c r="L163" s="103"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="17">
         <v>163</v>
       </c>
@@ -11323,7 +11324,7 @@
       <c r="K164" s="20"/>
       <c r="L164" s="103"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="17">
         <v>164</v>
       </c>
@@ -11405,7 +11406,7 @@
       <c r="K167" s="20"/>
       <c r="L167" s="103"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="17">
         <v>167</v>
       </c>
@@ -11433,7 +11434,7 @@
       <c r="K168" s="20"/>
       <c r="L168" s="103"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="17">
         <v>167</v>
       </c>
@@ -11463,7 +11464,7 @@
       <c r="K169" s="24"/>
       <c r="L169" s="103"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="17">
         <v>168</v>
       </c>
@@ -11523,7 +11524,7 @@
       <c r="K171" s="24"/>
       <c r="L171" s="103"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="17">
         <v>170</v>
       </c>
@@ -11553,7 +11554,7 @@
       <c r="K172" s="25"/>
       <c r="L172" s="103"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="17">
         <v>171</v>
       </c>
@@ -11583,7 +11584,7 @@
       <c r="K173" s="25"/>
       <c r="L173" s="103"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="17">
         <v>172</v>
       </c>
@@ -11611,7 +11612,7 @@
       <c r="K174" s="25"/>
       <c r="L174" s="103"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="17">
         <v>173</v>
       </c>
@@ -11639,7 +11640,7 @@
       <c r="K175" s="25"/>
       <c r="L175" s="103"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="17">
         <v>174</v>
       </c>
@@ -11699,7 +11700,7 @@
       <c r="K177" s="25"/>
       <c r="L177" s="103"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="17">
         <v>176</v>
       </c>
@@ -11729,7 +11730,7 @@
       <c r="K178" s="130"/>
       <c r="L178" s="103"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="17">
         <v>176</v>
       </c>
@@ -15016,7 +15017,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L318" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}"/>
+  <autoFilter ref="A1:L318" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" xr:uid="{C4DE44B4-9E86-4104-81E3-C93D60F64BE3}"/>
     <hyperlink ref="L2" r:id="rId2" xr:uid="{A4124D5F-F457-4A70-A072-5DFAF5EA33F8}"/>
@@ -71762,12 +71769,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -72005,18 +72012,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -72042,11 +72051,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>